<commit_message>
Fixed B06 test to gnomio
</commit_message>
<xml_diff>
--- a/CO3015_Assignment3/resource/B06_data.xlsx
+++ b/CO3015_Assignment3/resource/B06_data.xlsx
@@ -16,25 +16,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>TC-B05-001</t>
-  </si>
-  <si>
     <t>Testcase ID</t>
   </si>
   <si>
-    <t>data-conversation-id</t>
+    <t>TC-B06-001</t>
   </si>
   <si>
-    <t>TC-B05-002,
-TC-B05-003,
-TC-B05-004</t>
+    <t>TC-B06-002,
+TC-B06-003,
+TC-B06-004</t>
+  </si>
+  <si>
+    <t>data-user-id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +44,18 @@
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -69,14 +81,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -385,37 +399,38 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>66963</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
+    <row r="3" spans="1:2" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>233963</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.8" x14ac:dyDescent="0.3">

</xml_diff>